<commit_message>
Reads line by line from procedure file
</commit_message>
<xml_diff>
--- a/Data/Procedures/imagemap.xlsx
+++ b/Data/Procedures/imagemap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andywang/Desktop/Learning Behavior/Aliens/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andywang/Desktop/Preston Lab/Aliens/Data/Procedures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009D7F4C-1C93-9A45-89F2-E557EBCBEC0F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE2BE19-EC60-6844-9FBE-4FEFE2C85368}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23260" windowHeight="12580" xr2:uid="{BD53F7A6-3B44-6D46-90D6-01272792EFD4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="141">
   <si>
     <t>ID</t>
   </si>
@@ -39,21 +39,6 @@
     <t>Image Path</t>
   </si>
   <si>
-    <t>context_1</t>
-  </si>
-  <si>
-    <t>context_2</t>
-  </si>
-  <si>
-    <t>context_3</t>
-  </si>
-  <si>
-    <t>context_4</t>
-  </si>
-  <si>
-    <t>context_5</t>
-  </si>
-  <si>
     <t>1_tail_1</t>
   </si>
   <si>
@@ -82,9 +67,6 @@
   </si>
   <si>
     <t>1_gloves_5</t>
-  </si>
-  <si>
-    <t>Data/Images/brain.png</t>
   </si>
   <si>
     <t>1_body</t>
@@ -829,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D65F7A-FAAB-B447-AB7C-735700654342}">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -852,602 +834,562 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B40" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B56" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B57" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B59" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B67" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B68" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B69" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>2</v>
-      </c>
-      <c r="B72" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>3</v>
-      </c>
-      <c r="B73" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>4</v>
-      </c>
-      <c r="B74" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>5</v>
-      </c>
-      <c r="B75" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>6</v>
-      </c>
-      <c r="B76" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>